<commit_message>
Using more reasonable initial guesses in ExampleProblem.xlsx.
</commit_message>
<xml_diff>
--- a/ExampleProblem.xlsx
+++ b/ExampleProblem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="12435" windowHeight="9465" tabRatio="827"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="12432" windowHeight="9468" tabRatio="827"/>
   </bookViews>
   <sheets>
     <sheet name="Problem Setup" sheetId="1" r:id="rId1"/>
@@ -770,11 +770,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1084,84 +1084,84 @@
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -1218,14 +1218,14 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1235,7 +1235,7 @@
       <c r="C17" s="3"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="H20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1329,7 +1329,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1350,7 +1350,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1359,7 +1359,7 @@
       <c r="D24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1497,13 +1497,13 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1569,12 +1569,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -1617,52 +1617,52 @@
         <v>65000</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>23</v>
       </c>
       <c r="B42" s="6">
-        <f>$C$18*EXP($E$18*B$41)</f>
+        <f t="shared" ref="B42:K42" si="0">$C$18*EXP($E$18*B$41)</f>
         <v>3</v>
       </c>
       <c r="C42" s="6">
-        <f>$C$18*EXP($E$18*C$41)</f>
+        <f t="shared" si="0"/>
         <v>3.0606040200802673</v>
       </c>
       <c r="D42" s="6">
-        <f>$C$18*EXP($E$18*D$41)</f>
+        <f t="shared" si="0"/>
         <v>3.1224323225771649</v>
       </c>
       <c r="E42" s="6">
-        <f>$C$18*EXP($E$18*E$41)</f>
+        <f t="shared" si="0"/>
         <v>3.1538132891280721</v>
       </c>
       <c r="F42" s="6">
-        <f>$C$18*EXP($E$18*F$41)</f>
+        <f t="shared" si="0"/>
         <v>3.2336524526538946</v>
       </c>
       <c r="G42" s="6">
-        <f>$C$18*EXP($E$18*G$41)</f>
+        <f t="shared" si="0"/>
         <v>3.3155127542269431</v>
       </c>
       <c r="H42" s="6">
-        <f>$C$18*EXP($E$18*H$41)</f>
+        <f t="shared" si="0"/>
         <v>3.6642082744805098</v>
       </c>
       <c r="I42" s="6">
-        <f>$C$18*EXP($E$18*I$41)</f>
+        <f t="shared" si="0"/>
         <v>4.0495764227280091</v>
       </c>
       <c r="J42" s="6">
-        <f>$C$18*EXP($E$18*J$41)</f>
+        <f t="shared" si="0"/>
         <v>4.9461638121003846</v>
       </c>
       <c r="K42" s="6">
-        <f>$C$18*EXP($E$18*K$41)</f>
+        <f t="shared" si="0"/>
         <v>5.7466224870416891</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -1691,44 +1691,44 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>25</v>
       </c>
       <c r="B44" s="6">
-        <f>$C$19*EXP($E$19*B$43)</f>
+        <f t="shared" ref="B44:I44" si="1">$C$19*EXP($E$19*B$43)</f>
         <v>1.5</v>
       </c>
       <c r="C44" s="6">
-        <f>$C$19*EXP($E$19*C$43)</f>
+        <f t="shared" si="1"/>
         <v>1.5456818009302755</v>
       </c>
       <c r="D44" s="6">
-        <f>$C$19*EXP($E$19*D$43)</f>
+        <f t="shared" si="1"/>
         <v>1.6168262263269473</v>
       </c>
       <c r="E44" s="6">
-        <f>$C$19*EXP($E$19*E$43)</f>
+        <f t="shared" si="1"/>
         <v>1.7427513640924246</v>
       </c>
       <c r="F44" s="6">
-        <f>$C$19*EXP($E$19*F$43)</f>
+        <f t="shared" si="1"/>
         <v>1.9068737254821071</v>
       </c>
       <c r="G44" s="6">
-        <f>$C$19*EXP($E$19*G$43)</f>
+        <f t="shared" si="1"/>
         <v>2.0247882113640046</v>
       </c>
       <c r="H44" s="6">
-        <f>$C$19*EXP($E$19*H$43)</f>
+        <f t="shared" si="1"/>
         <v>2.3524682782352535</v>
       </c>
       <c r="I44" s="6">
-        <f>$C$19*EXP($E$19*I$43)</f>
+        <f t="shared" si="1"/>
         <v>3.1755000249190122</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>18</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -1768,48 +1768,48 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>21</v>
       </c>
       <c r="B47" s="6">
-        <f>$C$21*EXP(-$E$21*B$46)</f>
+        <f t="shared" ref="B47:J47" si="2">$C$21*EXP(-$E$21*B$46)</f>
         <v>15</v>
       </c>
       <c r="C47" s="6">
-        <f>$C$21*EXP(-$E$21*C$46)</f>
+        <f t="shared" si="2"/>
         <v>12.78215683449317</v>
       </c>
       <c r="D47" s="6">
-        <f>$C$21*EXP(-$E$21*D$46)</f>
+        <f t="shared" si="2"/>
         <v>10.892235556105364</v>
       </c>
       <c r="E47" s="6">
-        <f>$C$21*EXP(-$E$21*E$46)</f>
+        <f t="shared" si="2"/>
         <v>8.2321745414103962</v>
       </c>
       <c r="F47" s="6">
-        <f>$C$21*EXP(-$E$21*F$46)</f>
+        <f t="shared" si="2"/>
         <v>6.7399344617583239</v>
       </c>
       <c r="G47" s="6">
-        <f>$C$21*EXP(-$E$21*G$46)</f>
+        <f t="shared" si="2"/>
         <v>4.5179131786830302</v>
       </c>
       <c r="H47" s="6">
-        <f>$C$21*EXP(-$E$21*H$46)</f>
+        <f t="shared" si="2"/>
         <v>3.0284477699198309</v>
       </c>
       <c r="I47" s="6">
-        <f>$C$21*EXP(-$E$21*I$46)</f>
+        <f t="shared" si="2"/>
         <v>1.3607692993411871</v>
       </c>
       <c r="J47" s="6">
-        <f>$C$21*EXP(-$E$21*J$46)</f>
+        <f t="shared" si="2"/>
         <v>0.61143305967549322</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -1832,36 +1832,36 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>27</v>
       </c>
       <c r="B49" s="6">
-        <f>$C$22*EXP(-$E$22*B$48)</f>
+        <f t="shared" ref="B49:G49" si="3">$C$22*EXP(-$E$22*B$48)</f>
         <v>10</v>
       </c>
       <c r="C49" s="6">
-        <f>$C$22*EXP(-$E$22*C$48)</f>
+        <f t="shared" si="3"/>
         <v>8.6070797642505781</v>
       </c>
       <c r="D49" s="6">
-        <f>$C$22*EXP(-$E$22*D$48)</f>
+        <f t="shared" si="3"/>
         <v>6.8728927879097226</v>
       </c>
       <c r="E49" s="6">
-        <f>$C$22*EXP(-$E$22*E$48)</f>
+        <f t="shared" si="3"/>
         <v>5.3526142851899028</v>
       </c>
       <c r="F49" s="6">
-        <f>$C$22*EXP(-$E$22*F$48)</f>
+        <f t="shared" si="3"/>
         <v>3.6787944117144233</v>
       </c>
       <c r="G49" s="6">
-        <f>$C$22*EXP(-$E$22*G$48)</f>
+        <f t="shared" si="3"/>
         <v>2.2313016014842981</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -1887,40 +1887,40 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>29</v>
       </c>
       <c r="B51" s="6">
-        <f>$C$23*EXP(-$E$23*B$50)</f>
+        <f t="shared" ref="B51:H51" si="4">$C$23*EXP(-$E$23*B$50)</f>
         <v>25</v>
       </c>
       <c r="C51" s="6">
-        <f>$C$23*EXP(-$E$23*C$50)</f>
+        <f t="shared" si="4"/>
         <v>19.470019576785123</v>
       </c>
       <c r="D51" s="6">
-        <f>$C$23*EXP(-$E$23*D$50)</f>
+        <f t="shared" si="4"/>
         <v>15.163266492815836</v>
       </c>
       <c r="E51" s="6">
-        <f>$C$23*EXP(-$E$23*E$50)</f>
+        <f t="shared" si="4"/>
         <v>9.1969860292860588</v>
       </c>
       <c r="F51" s="6">
-        <f>$C$23*EXP(-$E$23*F$50)</f>
+        <f t="shared" si="4"/>
         <v>5.5782540037107458</v>
       </c>
       <c r="G51" s="6">
-        <f>$C$23*EXP(-$E$23*G$50)</f>
+        <f t="shared" si="4"/>
         <v>2.05212496559747</v>
       </c>
       <c r="H51" s="6">
-        <f>$C$23*EXP(-$E$23*H$50)</f>
+        <f t="shared" si="4"/>
         <v>0.75493458555796256</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>10</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>30</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -1963,31 +1963,31 @@
         <v>0</v>
       </c>
       <c r="C54" s="9">
-        <f t="shared" ref="C54:H54" si="0">MAX($E$25*C$53*(1-EXP(-$C$25*C$53))-$G$25,0)</f>
+        <f t="shared" ref="C54:H54" si="5">MAX($E$25*C$53*(1-EXP(-$C$25*C$53))-$G$25,0)</f>
         <v>2660.6027941427883</v>
       </c>
       <c r="D54" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8146.6471676338733</v>
       </c>
       <c r="E54" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>13753.193974482041</v>
       </c>
       <c r="F54" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>19133.687222225315</v>
       </c>
       <c r="G54" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>29425.637434700009</v>
       </c>
       <c r="H54" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>39486.581494883896</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -2011,7 +2011,7 @@
       </c>
       <c r="H55" s="9"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -2020,28 +2020,28 @@
         <v>0</v>
       </c>
       <c r="C56" s="7">
-        <f t="shared" ref="C56:G56" si="1">MAX($E$28*C$55*(1-EXP(-$C$28*C$55))-$G$28,0)</f>
+        <f t="shared" ref="C56:G56" si="6">MAX($E$28*C$55*(1-EXP(-$C$28*C$55))-$G$28,0)</f>
         <v>0</v>
       </c>
       <c r="D56" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1389.7711161949196</v>
       </c>
       <c r="E56" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>6274.6820696598734</v>
       </c>
       <c r="F56" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11865.888926202295</v>
       </c>
       <c r="G56" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>17514.528435713321</v>
       </c>
       <c r="H56" s="9"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>43000</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -2076,31 +2076,31 @@
         <v>0</v>
       </c>
       <c r="C58" s="7">
-        <f t="shared" ref="C58:H58" si="2">MAX($E$26*C$57*(1-EXP(-$C$26*C$57))-$G$26,0)</f>
+        <f t="shared" ref="C58:H58" si="7">MAX($E$26*C$57*(1-EXP(-$C$26*C$57))-$G$26,0)</f>
         <v>1467.346701436833</v>
       </c>
       <c r="D58" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>5821.2055882855766</v>
       </c>
       <c r="E58" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>13958.95598961721</v>
       </c>
       <c r="F58" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>22447.875034402528</v>
       </c>
       <c r="G58" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>33443.091580218854</v>
       </c>
       <c r="H58" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>41916.551962475365</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>30</v>
       </c>
@@ -2138,7 +2138,7 @@
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -2154,7 +2154,7 @@
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>31</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -2189,31 +2189,31 @@
         <v>0</v>
       </c>
       <c r="C64" s="7">
-        <f t="shared" ref="C64:H64" si="3">MAX($E$30*C$63*(1-EXP(-$C$30*C$63))-$G$30,0)</f>
+        <f t="shared" ref="C64:H64" si="8">MAX($E$30*C$63*(1-EXP(-$C$30*C$63))-$G$30,0)</f>
         <v>302.99804232148779</v>
       </c>
       <c r="D64" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1717.346701436833</v>
       </c>
       <c r="E64" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3707.2508544423899</v>
       </c>
       <c r="F64" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>6071.2055882855766</v>
       </c>
       <c r="G64" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>11403.047597773553</v>
       </c>
       <c r="H64" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>14208.95598961721</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>19</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>32</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>39</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>40</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>43000</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>37</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>38</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>43</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>44</v>
       </c>
@@ -2365,17 +2365,17 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>58</v>
       </c>
@@ -2383,12 +2383,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
         <v>61</v>
       </c>
@@ -2419,7 +2419,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -2600,7 +2600,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -2866,7 +2866,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -3313,7 +3313,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -3534,19 +3534,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>10050.640386179501</v>
+        <v>10000</v>
       </c>
       <c r="B1">
-        <v>11312.9692076274</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>22028.156015179</v>
+        <v>15000</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>13684.530792372499</v>
+        <v>15000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>